<commit_message>
new xlsx inputs for spain and france
</commit_message>
<xml_diff>
--- a/4_HealthEconomics/Inputs/provider_cost_inputs.xlsx
+++ b/4_HealthEconomics/Inputs/provider_cost_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Federated Analysis - Post-menopausal fracture\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/orms0952_ox_ac_uk/Documents/Documents/GitHub/RefractureStudy/4_HealthEconomics/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41567F39-FC66-49DD-B29B-88D4E827CAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A193161-AFDF-4AFC-93D5-E85BAE8E0418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="20832" windowHeight="16656" tabRatio="798" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9675" yWindow="2955" windowWidth="19230" windowHeight="11295" tabRatio="798" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="236">
   <si>
     <t>specialty_source_value</t>
   </si>
@@ -748,6 +748,9 @@
   </si>
   <si>
     <t>Dentist Anesthesiologist</t>
+  </si>
+  <si>
+    <t>Not assigned</t>
   </si>
 </sst>
 </file>
@@ -1156,15 +1159,15 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" style="6"/>
+    <col min="1" max="1" width="47.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
     <col min="3" max="3" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.54296875" style="6"/>
+    <col min="4" max="16384" width="8.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1178,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1209,7 +1212,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -1253,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
@@ -1300,7 +1303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
@@ -1308,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
@@ -1339,7 +1342,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>23</v>
       </c>
@@ -1378,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>24</v>
       </c>
@@ -1386,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>25</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>26</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>27</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>29</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>30</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>31</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
@@ -1469,7 +1472,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>33</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>34</v>
       </c>
@@ -1488,7 +1491,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>35</v>
       </c>
@@ -1496,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>36</v>
       </c>
@@ -1504,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>37</v>
       </c>
@@ -1512,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>38</v>
       </c>
@@ -1520,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>39</v>
       </c>
@@ -1528,7 +1531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>40</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>41</v>
       </c>
@@ -1547,7 +1550,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>42</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>43</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>44</v>
       </c>
@@ -1575,7 +1578,7 @@
         <v>26.74540816326531</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>45</v>
       </c>
@@ -1587,7 +1590,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>46</v>
       </c>
@@ -1595,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>47</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>48</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>26.74540816326531</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>49</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>1</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
@@ -1647,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -1655,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>52</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -1674,7 +1677,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>30.741666666666667</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>55</v>
       </c>
@@ -1697,7 +1700,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>56</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>30.741666666666667</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>57</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>30.741666666666667</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>58</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>59</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>30.741666666666667</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>60</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>62</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>63</v>
       </c>
@@ -1777,7 +1780,7 @@
         <v>30.741666666666667</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>64</v>
       </c>
@@ -1788,7 +1791,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>65</v>
       </c>
@@ -1799,7 +1802,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
@@ -1807,12 +1810,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>67</v>
       </c>
@@ -1820,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>68</v>
       </c>
@@ -1828,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>69</v>
       </c>
@@ -1836,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>70</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>30.741666666666667</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>71</v>
       </c>
@@ -1860,7 +1863,7 @@
         <v>26.74540816326531</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>72</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>73</v>
       </c>
@@ -1879,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>74</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>75</v>
       </c>
@@ -1895,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>76</v>
       </c>
@@ -1903,7 +1906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>77</v>
       </c>
@@ -1914,7 +1917,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>78</v>
       </c>
@@ -1922,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>79</v>
       </c>
@@ -1930,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>80</v>
       </c>
@@ -1941,7 +1944,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>81</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>82</v>
       </c>
@@ -1960,7 +1963,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>83</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>84</v>
       </c>
@@ -1983,7 +1986,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>85</v>
       </c>
@@ -1995,7 +1998,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>86</v>
       </c>
@@ -2006,7 +2009,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>87</v>
       </c>
@@ -2018,7 +2021,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>2</v>
       </c>
@@ -2029,7 +2032,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>88</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>89</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>90</v>
       </c>
@@ -2056,7 +2059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>91</v>
       </c>
@@ -2067,7 +2070,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>92</v>
       </c>
@@ -2078,7 +2081,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>93</v>
       </c>
@@ -2086,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>94</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>95</v>
       </c>
@@ -2105,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>96</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>97</v>
       </c>
@@ -2128,7 +2131,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>98</v>
       </c>
@@ -2140,7 +2143,7 @@
         <v>26.75</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>99</v>
       </c>
@@ -2151,7 +2154,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>100</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>101</v>
       </c>
@@ -2170,7 +2173,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>102</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>103</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>104</v>
       </c>
@@ -2200,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>105</v>
       </c>
@@ -2212,7 +2215,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>106</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>107</v>
       </c>
@@ -2228,7 +2231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>108</v>
       </c>
@@ -2236,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>109</v>
       </c>
@@ -2247,7 +2250,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>110</v>
       </c>
@@ -2258,7 +2261,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>111</v>
       </c>
@@ -2266,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>112</v>
       </c>
@@ -2274,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>113</v>
       </c>
@@ -2282,7 +2285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>114</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>115</v>
       </c>
@@ -2298,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>116</v>
       </c>
@@ -2310,7 +2313,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>117</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>118</v>
       </c>
@@ -2333,7 +2336,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>119</v>
       </c>
@@ -2344,7 +2347,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>120</v>
       </c>
@@ -2352,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>121</v>
       </c>
@@ -2364,7 +2367,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>122</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>123</v>
       </c>
@@ -2386,7 +2389,7 @@
         <v>107.26</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>124</v>
       </c>
@@ -2394,7 +2397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>125</v>
       </c>
@@ -2406,7 +2409,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>126</v>
       </c>
@@ -2417,7 +2420,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>127</v>
       </c>
@@ -2428,7 +2431,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>128</v>
       </c>
@@ -2440,7 +2443,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>129</v>
       </c>
@@ -2448,7 +2451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>130</v>
       </c>
@@ -2456,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>131</v>
       </c>
@@ -2467,7 +2470,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>132</v>
       </c>
@@ -2475,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>133</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>30.741666666666667</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>134</v>
       </c>
@@ -2499,7 +2502,7 @@
         <v>35.728813559322035</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>135</v>
       </c>
@@ -2507,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>136</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>137</v>
       </c>
@@ -2526,7 +2529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>138</v>
       </c>
@@ -2534,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>139</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>140</v>
       </c>
@@ -2550,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>141</v>
       </c>
@@ -2558,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>142</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>143</v>
       </c>
@@ -2581,7 +2584,7 @@
         <v>156.82</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>144</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>145</v>
       </c>
@@ -2600,7 +2603,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>146</v>
       </c>
@@ -2608,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>147</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>148</v>
       </c>
@@ -2624,7 +2627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>149</v>
       </c>
@@ -2635,7 +2638,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>150</v>
       </c>
@@ -2643,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>151</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>152</v>
       </c>
@@ -2665,7 +2668,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>153</v>
       </c>
@@ -2676,7 +2679,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
         <v>154</v>
       </c>
@@ -2687,7 +2690,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
         <v>155</v>
       </c>
@@ -2698,7 +2701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>156</v>
       </c>
@@ -2706,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
         <v>157</v>
       </c>
@@ -2717,7 +2720,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
         <v>158</v>
       </c>
@@ -2728,7 +2731,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
         <v>159</v>
       </c>
@@ -2736,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
         <v>160</v>
       </c>
@@ -2744,7 +2747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
         <v>161</v>
       </c>
@@ -2756,7 +2759,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
         <v>162</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
         <v>163</v>
       </c>
@@ -2779,7 +2782,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
         <v>164</v>
       </c>
@@ -2787,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
         <v>165</v>
       </c>
@@ -2795,7 +2798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
         <v>166</v>
       </c>
@@ -2803,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
         <v>167</v>
       </c>
@@ -2811,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
         <v>168</v>
       </c>
@@ -2823,7 +2826,7 @@
         <v>26.74540816326531</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
         <v>169</v>
       </c>
@@ -2835,7 +2838,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
         <v>170</v>
       </c>
@@ -2843,7 +2846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
         <v>171</v>
       </c>
@@ -2851,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
         <v>172</v>
       </c>
@@ -2859,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
         <v>173</v>
       </c>
@@ -2870,7 +2873,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
         <v>174</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
         <v>175</v>
       </c>
@@ -2886,7 +2889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
         <v>176</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
         <v>177</v>
       </c>
@@ -2905,7 +2908,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
         <v>178</v>
       </c>
@@ -2913,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
         <v>179</v>
       </c>
@@ -2924,7 +2927,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
         <v>180</v>
       </c>
@@ -2935,7 +2938,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="6" t="s">
         <v>181</v>
       </c>
@@ -2946,7 +2949,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
         <v>182</v>
       </c>
@@ -2954,7 +2957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="6" t="s">
         <v>183</v>
       </c>
@@ -2965,7 +2968,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
         <v>184</v>
       </c>
@@ -2973,7 +2976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="6" t="s">
         <v>185</v>
       </c>
@@ -2984,7 +2987,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
         <v>186</v>
       </c>
@@ -2996,7 +2999,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="6" t="s">
         <v>187</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="6" t="s">
         <v>188</v>
       </c>
@@ -3012,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="6" t="s">
         <v>189</v>
       </c>
@@ -3020,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="6" t="s">
         <v>190</v>
       </c>
@@ -3031,7 +3034,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="6" t="s">
         <v>191</v>
       </c>
@@ -3043,7 +3046,7 @@
         <v>19.196153846153848</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
         <v>192</v>
       </c>
@@ -3051,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="6" t="s">
         <v>193</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="6" t="s">
         <v>194</v>
       </c>
@@ -3070,7 +3073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="6" t="s">
         <v>195</v>
       </c>
@@ -3078,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="6" t="s">
         <v>196</v>
       </c>
@@ -3086,7 +3089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
         <v>197</v>
       </c>
@@ -3111,12 +3114,12 @@
       <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3127,7 +3130,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>200</v>
       </c>
@@ -3151,13 +3154,13 @@
       <selection activeCell="D1" sqref="D1:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>201</v>
       </c>
@@ -3171,7 +3174,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>38004451</v>
       </c>
@@ -3185,7 +3188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>45756756</v>
       </c>
@@ -3199,7 +3202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>38004452</v>
       </c>
@@ -3213,7 +3216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>44777680</v>
       </c>
@@ -3227,7 +3230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>38004455</v>
       </c>
@@ -3241,7 +3244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>38004446</v>
       </c>
@@ -3255,7 +3258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>38004458</v>
       </c>
@@ -3269,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>38004505</v>
       </c>
@@ -3283,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>38004461</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>38004465</v>
       </c>
@@ -3311,7 +3314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>38004449</v>
       </c>
@@ -3325,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>38004477</v>
       </c>
@@ -3339,7 +3342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>38004469</v>
       </c>
@@ -3353,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>44777741</v>
       </c>
@@ -3367,7 +3370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>38004472</v>
       </c>
@@ -3381,7 +3384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>38004491</v>
       </c>
@@ -3395,7 +3398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>38004474</v>
       </c>
@@ -3421,18 +3424,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF16AF3-5FE4-4E51-A040-3A1DA41F7069}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="25.54296875" customWidth="1"/>
+    <col min="1" max="3" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>201</v>
       </c>
@@ -3446,7 +3449,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>38004451</v>
       </c>
@@ -3460,7 +3463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>38004452</v>
       </c>
@@ -3474,7 +3477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>44777680</v>
       </c>
@@ -3488,7 +3491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>38004455</v>
       </c>
@@ -3502,7 +3505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>38004446</v>
       </c>
@@ -3516,7 +3519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>38003902</v>
       </c>
@@ -3530,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>38004458</v>
       </c>
@@ -3544,7 +3547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>38004463</v>
       </c>
@@ -3558,18 +3561,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>38004477</v>
       </c>
       <c r="B10" t="s">
         <v>211</v>
       </c>
+      <c r="C10">
+        <v>26.5</v>
+      </c>
       <c r="D10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>38004469</v>
       </c>
@@ -3583,7 +3589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>38004472</v>
       </c>
@@ -3597,7 +3603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>38004491</v>
       </c>
@@ -3608,6 +3614,20 @@
         <v>26.5</v>
       </c>
       <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14" s="8">
+        <v>36.839090909090913</v>
+      </c>
+      <c r="D14">
         <v>1</v>
       </c>
     </row>
@@ -3623,19 +3643,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB2F280-3407-4F3E-A693-5661C6A1B47C}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1796875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>201</v>
       </c>
@@ -3649,7 +3669,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>38004446</v>
       </c>
@@ -3663,7 +3683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>38004385</v>
       </c>
@@ -3677,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>38004477</v>
       </c>
@@ -3691,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>38004510</v>
       </c>
@@ -3705,7 +3725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>38004482</v>
       </c>
@@ -3719,7 +3739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>38004461</v>
       </c>
@@ -3733,7 +3753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>43125856</v>
       </c>
@@ -3747,7 +3767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>38004499</v>
       </c>
@@ -3761,7 +3781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>38004452</v>
       </c>
@@ -3775,7 +3795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>38004474</v>
       </c>
@@ -3789,7 +3809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>38004472</v>
       </c>
@@ -3800,6 +3820,20 @@
         <v>61.636146898938016</v>
       </c>
       <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="8">
+        <v>57.405918307512138</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
     </row>
@@ -3819,13 +3853,13 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>223</v>
       </c>
@@ -3836,7 +3870,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>262</v>
       </c>
@@ -3847,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9201</v>
       </c>
@@ -3858,7 +3892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9202</v>
       </c>
@@ -3869,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9203</v>
       </c>
@@ -3880,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>581476</v>
       </c>
@@ -3897,15 +3931,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E261632A9079424993A897DC15346D5B" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e142ea7856c1c779e772802f85df3c9d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1fd57a85-5f09-446c-9d29-22a13ed0863b" xmlns:ns3="47a2ec26-e196-46c3-886b-68c32d2bf91e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="08527c5e4e22af13f6da42aeeb5331bb" ns2:_="" ns3:_="">
     <xsd:import namespace="1fd57a85-5f09-446c-9d29-22a13ed0863b"/>
@@ -4154,15 +4179,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A041A22-800E-42F0-9103-7570B9474B4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDAB7EB0-42CF-45C9-9ECF-1747D13501DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4179,4 +4205,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A041A22-800E-42F0-9103-7570B9474B4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>